<commit_message>
Pequenas alteracoes em documentos
</commit_message>
<xml_diff>
--- a/CCG - ENFIAÇÃO AUTOMAÇÃO FALADA.xlsx
+++ b/CCG - ENFIAÇÃO AUTOMAÇÃO FALADA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toniezzer-PC\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Downloads\Guila-s-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{35293013-25DD-4908-B7CC-A009276C5653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1887F15-424C-4BD1-9FD3-D56C98110E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{DB79FB51-86ED-4568-B032-71F843597583}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{DB79FB51-86ED-4568-B032-71F843597583}"/>
   </bookViews>
   <sheets>
     <sheet name="PAVIMENTO INFERIOR" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="97">
   <si>
     <t>GARAGEM</t>
   </si>
@@ -287,6 +287,36 @@
   </si>
   <si>
     <t>HALL SUPERIOR</t>
+  </si>
+  <si>
+    <t>1S</t>
+  </si>
+  <si>
+    <t>RESERVA, FICA EM CIMA DA MESA</t>
+  </si>
+  <si>
+    <t>220V</t>
+  </si>
+  <si>
+    <t>AINDA NÃO DEFINIDO</t>
+  </si>
+  <si>
+    <t>2J</t>
+  </si>
+  <si>
+    <t>RESERVA</t>
+  </si>
+  <si>
+    <t>ARANDELA PORTA LAVABO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXISTE OUTRO CIRCUITO CHAMADAO 'K2.' VER O QUE É </t>
+  </si>
+  <si>
+    <t>2K.</t>
+  </si>
+  <si>
+    <t>VER O QUE É</t>
   </si>
 </sst>
 </file>
@@ -344,7 +374,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -368,6 +398,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -745,22 +778,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55976542-2843-4B6C-A8B9-799624AB2111}">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="G46" sqref="E41:G46"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36:C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="26.5703125" customWidth="1"/>
-    <col min="5" max="5" width="32.5703125" customWidth="1"/>
-    <col min="6" max="6" width="26.5703125" customWidth="1"/>
-    <col min="7" max="7" width="30.140625" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="26.5546875" customWidth="1"/>
+    <col min="5" max="5" width="32.5546875" customWidth="1"/>
+    <col min="6" max="6" width="26.5546875" customWidth="1"/>
+    <col min="7" max="7" width="30.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -783,7 +816,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -806,7 +839,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -829,7 +862,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
@@ -852,7 +885,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="C5" s="2">
@@ -869,7 +902,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="8"/>
       <c r="C6" s="2">
@@ -886,7 +919,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="8">
         <v>25</v>
@@ -905,7 +938,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="8"/>
       <c r="C8" s="2">
@@ -922,7 +955,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="2">
@@ -939,7 +972,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -962,7 +995,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -985,7 +1018,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
@@ -1008,7 +1041,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="2">
@@ -1025,7 +1058,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>34</v>
       </c>
@@ -1048,7 +1081,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="4">
         <v>34</v>
@@ -1067,7 +1100,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="4">
         <v>34</v>
@@ -1085,618 +1118,666 @@
       <c r="G16" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="H16" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="7"/>
+      <c r="B17" s="4">
+        <v>34</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B18" s="4">
         <v>33</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C18" s="2">
         <v>5</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B19" s="8">
         <v>35</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C19" s="2">
         <v>16</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="2">
-        <v>17</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="2">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="2">
+        <v>21</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="7"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="2">
         <v>22</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G24" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B25" s="8">
         <v>30</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C25" s="2">
         <v>16</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="2">
-        <v>17</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" s="8"/>
       <c r="C26" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="G26" s="7"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="2">
-        <v>19</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>49</v>
+        <v>18</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="B28" s="8"/>
       <c r="C28" s="2">
-        <v>20</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>53</v>
+        <v>19</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="8"/>
       <c r="C29" s="2">
+        <v>20</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="7"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="2">
         <v>21</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G30" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B31" s="8">
         <v>29</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C31" s="2">
         <v>12</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G31" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="2">
-        <v>13</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="8"/>
       <c r="C32" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
       <c r="B33" s="8"/>
       <c r="C33" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="7"/>
       <c r="B34" s="8"/>
       <c r="C34" s="2">
+        <v>15</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="7"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="2">
         <v>16</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G35" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B35" s="7">
+      <c r="B36" s="7">
         <v>26</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C36" s="9">
         <v>13</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="2">
-        <v>14</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
-      <c r="C37" s="2">
-        <v>15</v>
+      <c r="C37" s="9">
+        <v>14</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
-      <c r="C38" s="2">
-        <v>16</v>
+      <c r="C38" s="9">
+        <v>15</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
-      <c r="C39" s="2">
-        <v>17</v>
+      <c r="C39" s="9">
+        <v>16</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
-      <c r="C40" s="2">
+      <c r="C40" s="9">
+        <v>17</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D40" s="2">
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="9">
+        <v>50</v>
+      </c>
+      <c r="D41" s="2">
         <v>1</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F41" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="G41" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="7">
+      <c r="B42" s="7">
         <v>22</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C42" s="2">
         <v>13</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="2">
-        <v>14</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="2">
+        <v>17</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="7"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="2">
         <v>20</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2" t="s">
+      <c r="E47" s="2"/>
+      <c r="F47" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="G47" s="2" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="7"/>
+      <c r="B48" s="7"/>
+      <c r="D48" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D51" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E51" t="s">
+        <v>92</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="A25:A30"/>
+    <mergeCell ref="B25:B30"/>
+    <mergeCell ref="B31:B35"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="B36:B41"/>
+    <mergeCell ref="A36:A41"/>
+    <mergeCell ref="A42:A48"/>
+    <mergeCell ref="B42:B48"/>
+    <mergeCell ref="B19:B24"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="E14:E17"/>
     <mergeCell ref="E4:E9"/>
     <mergeCell ref="E12:E13"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="A14:A16"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="A24:A29"/>
-    <mergeCell ref="B24:B29"/>
-    <mergeCell ref="A41:A46"/>
-    <mergeCell ref="B41:B46"/>
-    <mergeCell ref="B30:B34"/>
-    <mergeCell ref="A30:A34"/>
-    <mergeCell ref="B35:B40"/>
-    <mergeCell ref="A35:A40"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1711,16 +1792,16 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="26.5703125" customWidth="1"/>
-    <col min="4" max="4" width="32.5703125" customWidth="1"/>
-    <col min="5" max="6" width="26.5703125" customWidth="1"/>
-    <col min="7" max="7" width="30.140625" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="26.5546875" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" customWidth="1"/>
+    <col min="5" max="6" width="26.5546875" customWidth="1"/>
+    <col min="7" max="7" width="30.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -1743,7 +1824,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>86</v>
       </c>
@@ -1766,7 +1847,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="4"/>
       <c r="C3" s="2">
@@ -1777,7 +1858,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="5"/>
       <c r="C4" s="2"/>
@@ -1786,7 +1867,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="5"/>
       <c r="C5" s="2"/>
@@ -1795,7 +1876,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="5"/>
       <c r="C6" s="2"/>
@@ -1804,7 +1885,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="5"/>
       <c r="C7" s="2"/>
@@ -1813,7 +1894,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="5"/>
       <c r="C8" s="2"/>
@@ -1822,7 +1903,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="5"/>
       <c r="C9" s="2"/>
@@ -1831,7 +1912,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="4"/>
       <c r="C10" s="2"/>
@@ -1840,7 +1921,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="2"/>
@@ -1849,7 +1930,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
       <c r="C12" s="2"/>
@@ -1858,7 +1939,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="5"/>
       <c r="C13" s="2"/>
@@ -1867,7 +1948,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="2"/>
@@ -1876,7 +1957,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="2"/>
@@ -1885,7 +1966,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="2"/>
@@ -1894,7 +1975,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
       <c r="C17" s="2"/>
@@ -1903,7 +1984,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="5"/>
       <c r="C18" s="2"/>
@@ -1912,7 +1993,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="5"/>
       <c r="C19" s="2"/>
@@ -1921,7 +2002,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="5"/>
       <c r="C20" s="2"/>
@@ -1930,7 +2011,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="5"/>
       <c r="C21" s="2"/>
@@ -1939,7 +2020,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="5"/>
       <c r="C22" s="2"/>
@@ -1948,7 +2029,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="5"/>
       <c r="C23" s="2"/>
@@ -1957,7 +2038,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="5"/>
       <c r="C24" s="2"/>
@@ -1966,7 +2047,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="5"/>
       <c r="C25" s="2"/>
@@ -1975,7 +2056,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="5"/>
       <c r="C26" s="2"/>
@@ -1984,7 +2065,7 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="5"/>
       <c r="C27" s="2"/>
@@ -1993,7 +2074,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="5"/>
       <c r="C28" s="2"/>
@@ -2002,7 +2083,7 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="5"/>
       <c r="C29" s="2"/>
@@ -2011,7 +2092,7 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="5"/>
       <c r="C30" s="2"/>
@@ -2020,7 +2101,7 @@
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="5"/>
       <c r="C31" s="2"/>
@@ -2029,7 +2110,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="5"/>
       <c r="C32" s="2"/>
@@ -2038,7 +2119,7 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="5"/>
       <c r="C33" s="2"/>
@@ -2047,7 +2128,7 @@
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="5"/>
       <c r="C34" s="2"/>
@@ -2056,7 +2137,7 @@
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="2"/>
@@ -2065,7 +2146,7 @@
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="2"/>
@@ -2074,7 +2155,7 @@
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="2"/>
@@ -2083,7 +2164,7 @@
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="2"/>
@@ -2092,7 +2173,7 @@
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="2"/>
@@ -2101,7 +2182,7 @@
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="2"/>
@@ -2110,7 +2191,7 @@
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="2"/>
@@ -2119,7 +2200,7 @@
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="2"/>
@@ -2128,7 +2209,7 @@
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="2"/>
@@ -2137,7 +2218,7 @@
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="2"/>
@@ -2146,7 +2227,7 @@
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="2"/>
@@ -2155,7 +2236,7 @@
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="2"/>

</xml_diff>